<commit_message>
finilizing mechanical design 3
</commit_message>
<xml_diff>
--- a/Mechanical Design/BOM.xlsx
+++ b/Mechanical Design/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Avid\avid-mech245\Mechanical Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEAFA66-011A-4E91-9D34-B17CA722248E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE1E507-4F9C-445B-B26B-72E47B01B2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>name</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>20mm</t>
+  </si>
+  <si>
+    <t>gripper</t>
+  </si>
+  <si>
+    <t>tool</t>
   </si>
 </sst>
 </file>
@@ -266,12 +272,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -279,9 +279,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="8" fontId="1" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -293,8 +290,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -577,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,397 +599,411 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
     </row>
     <row r="3" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="6">
         <v>58.08</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
     </row>
     <row r="4" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="7">
         <v>2</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="6">
         <v>89.54</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
     </row>
     <row r="5" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="7">
         <v>1</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="5">
         <v>14.39</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="7">
         <v>1</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="5">
         <v>5.0999999999999996</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
     </row>
     <row r="7" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="7">
         <v>4</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="5">
         <v>5.41</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="7">
         <v>4</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="5">
         <v>4.28</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
     </row>
     <row r="10" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="7">
         <v>1</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="5">
         <v>88.95</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="7">
         <v>1</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="5">
         <v>70.12</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
     </row>
     <row r="13" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="7">
         <v>2</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="5">
         <v>10.5</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="7">
         <v>2</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="5">
         <v>12.3</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="7">
         <v>1</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="5">
         <v>16.52</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="7">
         <v>2</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="5">
         <v>58.94</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="7">
         <v>2</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="5">
         <v>39.82</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5">
+        <v>14.99</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D21" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B22" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D22" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4" t="s">
+      <c r="B24" s="10"/>
+      <c r="C24" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+      <c r="D24" s="10"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7" t="s">
+      <c r="B25" s="8"/>
+      <c r="C25" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="7"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7" t="s">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7" t="s">
+      <c r="B27" s="8"/>
+      <c r="C27" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="7"/>
+      <c r="D27" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A23:D23"/>
     <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
     <mergeCell ref="G2:M9"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C24:D24"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C25:D25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" display="https://www.robotshop.com/eu/en/12v-17a-667oz-in-nema-17-bipolar-stepper-motor.html" xr:uid="{F1DBF49E-BAE0-4D28-9C1D-D655ECA598EA}"/>
@@ -999,8 +1019,9 @@
     <hyperlink ref="C15" r:id="rId11" display="$16.52" xr:uid="{F55CE233-AAEE-4E1C-8987-E4103F69630F}"/>
     <hyperlink ref="C16" r:id="rId12" display="$58.94" xr:uid="{DBD25648-8744-407E-9C63-17EC85290E7B}"/>
     <hyperlink ref="C17" r:id="rId13" display="$39.82" xr:uid="{2575C71D-19F8-4B98-88A2-23F70E761B6B}"/>
+    <hyperlink ref="C18" r:id="rId14" display="$14.99" xr:uid="{95828973-C934-45C5-BCE8-CB0F70F51B31}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId14"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>